<commit_message>
work deep 01 2023-04-21
</commit_message>
<xml_diff>
--- a/015 VBA Programming/08-01-form-controls.xlsx
+++ b/015 VBA Programming/08-01-form-controls.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web learning\015 VBA Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DD0FADA-B61D-4DA7-AFC9-CC1140F49DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{344C5022-0049-4B85-BAA4-5A3F5EEC6D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{0D1C013E-ACB1-4F51-B374-FE3A90D1DB47}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{0D1C013E-ACB1-4F51-B374-FE3A90D1DB47}"/>
   </bookViews>
   <sheets>
     <sheet name="Combo Box" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="42">
   <si>
     <t>Month</t>
   </si>
@@ -185,6 +185,9 @@
   </si>
   <si>
     <t>Clive</t>
+  </si>
+  <si>
+    <t>Vliamd</t>
   </si>
 </sst>
 </file>
@@ -298,6 +301,7 @@
     </font>
     <font>
       <sz val="8"/>
+      <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -552,7 +556,44 @@
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -627,7 +668,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="22" fmlaLink="$F$4" max="10" page="10" val="2"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="List" dx="22" fmlaLink="$B$13" fmlaRange="$M$5:$M$16" noThreeD="1" sel="5" val="0"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$B$5" max="10" min="1" page="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1173,7 +1218,7 @@
                   <a14:compatExt spid="_x0000_s3074"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75AB578C-3331-DB78-D3D6-13CD0EF5ABC5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-0000020C0000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1243,28 +1288,91 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
-          <xdr:colOff>371475</xdr:colOff>
+          <xdr:colOff>342900</xdr:colOff>
           <xdr:row>2</xdr:row>
-          <xdr:rowOff>38099</xdr:rowOff>
+          <xdr:rowOff>66675</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>1</xdr:col>
-          <xdr:colOff>657225</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>152399</xdr:rowOff>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>333375</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>133350</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="4097" name="Spinner 1" hidden="1">
+            <xdr:cNvPr id="4097" name="List Box 1" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s4097"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000001100000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000001100000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:noFill/>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>409576</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9524</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>542926</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>104774</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="5121" name="Scroll Bar 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s5121"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000001140000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1292,6 +1400,17 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D7475A6F-B868-4EC3-AD0D-F33549F0D67B}" name="Table1" displayName="Table1" ref="M4:N16" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="M4:N16" xr:uid="{D7475A6F-B868-4EC3-AD0D-F33549F0D67B}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{6E1E87A6-DD95-4A59-B33A-0EFCA479CA3E}" name="Employees"/>
+    <tableColumn id="2" xr3:uid="{07D5E713-AE21-419F-AECB-F52B7E47FF95}" name="Salary" dataDxfId="1" dataCellStyle="Comma"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1997,7 +2116,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C6:C16">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
       <formula>"Salary"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2042,7 +2161,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2287,12 +2406,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C8">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"Salary"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"Salary"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2353,12 +2472,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E384735-4872-4922-864B-16149C4AB987}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E384735-4872-4922-864B-16149C4AB987}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2391,13 +2510,8 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="23" t="str" cm="1">
-        <f t="array" ref="C4">INDEX(I4:I13,$F$4)</f>
-        <v>Claire</v>
-      </c>
-      <c r="F4" s="3">
-        <v>2</v>
-      </c>
+      <c r="C4" s="23"/>
+      <c r="F4" s="3"/>
       <c r="I4" t="s">
         <v>18</v>
       </c>
@@ -2425,10 +2539,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="25">
-        <f>VLOOKUP(C4,I4:J13,2,FALSE)</f>
-        <v>37941</v>
-      </c>
+      <c r="C7" s="25"/>
       <c r="I7" t="s">
         <v>21</v>
       </c>
@@ -2486,6 +2597,157 @@
     </row>
     <row r="22" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDDDD30-8B3A-4A34-8377-288875FD4AA0}">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="A1:N16"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="1.625" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.375" customWidth="1"/>
+    <col min="14" max="14" width="11.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21"/>
+      <c r="B1" s="22" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F3" s="31" cm="1">
+        <f t="array" ref="F3">INDEX(N5:N16,B13,1)</f>
+        <v>44061</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" s="5" t="str" cm="1">
+        <f t="array" ref="F4">"Salary for " &amp; INDEX(M5:M16,B13,1)</f>
+        <v>Salary for Adam</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>18</v>
+      </c>
+      <c r="N5" s="5">
+        <v>29750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" s="5">
+        <v>37941</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="5">
+        <v>21697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="5">
+        <v>34511</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="5">
+        <v>44061</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10" s="5">
+        <v>31727</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="5">
+        <v>47585</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="M12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N12" s="5">
+        <v>27273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B13" s="3">
+        <v>5</v>
+      </c>
+      <c r="M13" t="s">
+        <v>26</v>
+      </c>
+      <c r="N13" s="5">
+        <v>46133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M14" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="5">
+        <v>30043</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M15" t="s">
+        <v>18</v>
+      </c>
+      <c r="N15" s="5">
+        <v>12231</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M16" t="s">
+        <v>41</v>
+      </c>
+      <c r="N16" s="5">
+        <v>212</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2496,20 +2758,20 @@
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="4097" r:id="rId3" name="Spinner 1">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1" sizeWithCells="1">
+            <control shapeId="4097" r:id="rId3" name="List Box 1">
+              <controlPr defaultSize="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
                   <from>
                     <xdr:col>1</xdr:col>
-                    <xdr:colOff>371475</xdr:colOff>
+                    <xdr:colOff>342900</xdr:colOff>
                     <xdr:row>2</xdr:row>
-                    <xdr:rowOff>38100</xdr:rowOff>
+                    <xdr:rowOff>66675</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>1</xdr:col>
-                    <xdr:colOff>657225</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>333375</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>133350</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -2519,142 +2781,19 @@
       </controls>
     </mc:Choice>
   </mc:AlternateContent>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EDDDD30-8B3A-4A34-8377-288875FD4AA0}">
-  <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:N14"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="1.625" customWidth="1"/>
-    <col min="5" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" customWidth="1"/>
-    <col min="14" max="14" width="11.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" s="22" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="F3" s="31"/>
-    </row>
-    <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="F4" s="5"/>
-      <c r="M4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="5">
-        <v>29750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M6" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="5">
-        <v>37941</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="5">
-        <v>21697</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M8" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="5">
-        <v>34511</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M9" t="s">
-        <v>22</v>
-      </c>
-      <c r="N9" s="5">
-        <v>44061</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10" s="5">
-        <v>31727</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M11" t="s">
-        <v>24</v>
-      </c>
-      <c r="N11" s="5">
-        <v>47585</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="M12" t="s">
-        <v>25</v>
-      </c>
-      <c r="N12" s="5">
-        <v>27273</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="3"/>
-      <c r="M13" t="s">
-        <v>26</v>
-      </c>
-      <c r="N13" s="5">
-        <v>46133</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="M14" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="5">
-        <v>30043</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98F4DE6-C6C5-4166-8DCF-77A46886DD21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E98F4DE6-C6C5-4166-8DCF-77A46886DD21}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2686,6 +2825,9 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1</v>
+      </c>
       <c r="F5" s="37" t="s">
         <v>17</v>
       </c>
@@ -2697,6 +2839,14 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E6" t="str" cm="1">
+        <f t="array" ref="E6">IFERROR(INDEX(I5:$I$15,$B$5),"-")</f>
+        <v>Deb</v>
+      </c>
+      <c r="F6" cm="1">
+        <f t="array" ref="F6">IFERROR(INDEX(J5:$J$15,$B$5),"-")</f>
+        <v>29750</v>
+      </c>
       <c r="I6" t="s">
         <v>19</v>
       </c>
@@ -2705,6 +2855,14 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E7" t="str" cm="1">
+        <f t="array" ref="E7">IFERROR(INDEX(I6:$I$15,$B$5),"-")</f>
+        <v>Claire</v>
+      </c>
+      <c r="F7" cm="1">
+        <f t="array" ref="F7">IFERROR(INDEX(J6:$J$15,$B$5),"-")</f>
+        <v>37941</v>
+      </c>
       <c r="I7" t="s">
         <v>20</v>
       </c>
@@ -2713,6 +2871,14 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E8" t="str" cm="1">
+        <f t="array" ref="E8">IFERROR(INDEX(I7:$I$15,$B$5),"-")</f>
+        <v>Sam</v>
+      </c>
+      <c r="F8" cm="1">
+        <f t="array" ref="F8">IFERROR(INDEX(J7:$J$15,$B$5),"-")</f>
+        <v>21697</v>
+      </c>
       <c r="I8" t="s">
         <v>21</v>
       </c>
@@ -2721,6 +2887,14 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E9" t="str" cm="1">
+        <f t="array" ref="E9">IFERROR(INDEX(I8:$I$15,$B$5),"-")</f>
+        <v>Ben</v>
+      </c>
+      <c r="F9" cm="1">
+        <f t="array" ref="F9">IFERROR(INDEX(J8:$J$15,$B$5),"-")</f>
+        <v>34511</v>
+      </c>
       <c r="I9" t="s">
         <v>22</v>
       </c>
@@ -2729,6 +2903,14 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E10" t="str" cm="1">
+        <f t="array" ref="E10">IFERROR(INDEX(I9:$I$15,$B$5),"-")</f>
+        <v>Adam</v>
+      </c>
+      <c r="F10" cm="1">
+        <f t="array" ref="F10">IFERROR(INDEX(J9:$J$15,$B$5),"-")</f>
+        <v>44061</v>
+      </c>
       <c r="I10" t="s">
         <v>23</v>
       </c>
@@ -2779,5 +2961,35 @@
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="5121" r:id="rId3" name="Scroll Bar 1">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>409575</xdr:colOff>
+                    <xdr:row>5</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>542925</xdr:colOff>
+                    <xdr:row>14</xdr:row>
+                    <xdr:rowOff>104775</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
 </worksheet>
 </file>
</xml_diff>